<commit_message>
Update Solution_(3, 13, 3, 4, 3, 2, 2).xlsx
</commit_message>
<xml_diff>
--- a/Solution_(3, 13, 3, 4, 3, 2, 2).xlsx
+++ b/Solution_(3, 13, 3, 4, 3, 2, 2).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ncaandt-my.sharepoint.com/personal/jsadeghi_ncat_edu/Documents/ResearchPHD/00 PUBLISHED/2023 A JCP - Kia &amp; Moein Sus Resi/2022.06.28 Moein Codes/shared online/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ncaandt-my.sharepoint.com/personal/jsadeghi_ncat_edu/Documents/Documents/GitHub/Data2023JCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{BA3ADE10-99CC-46B4-BDD7-6085C1C1A17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18E046CB-D6A3-44C2-ACCC-9E973DE68F6D}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{BA3ADE10-99CC-46B4-BDD7-6085C1C1A17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF7AE8C9-6F68-4825-A122-D5D9ECC2A736}"/>
   <bookViews>
-    <workbookView xWindow="24468" yWindow="-108" windowWidth="24792" windowHeight="13320" xr2:uid="{6E5DFC6D-440D-4FE5-AC61-28AB0DAA08A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="24792" windowHeight="13320" xr2:uid="{6E5DFC6D-440D-4FE5-AC61-28AB0DAA08A1}"/>
   </bookViews>
   <sheets>
     <sheet name="(3, 13, 3, 4, 3, 2, 2)" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>z1</t>
   </si>
@@ -37,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Best</t>
   </si>
 </sst>
 </file>
@@ -52,12 +66,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +412,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,6 +427,15 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -416,6 +446,21 @@
       </c>
       <c r="C2">
         <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f>MIN(A:A)</f>
+        <v>957034.46581689897</v>
+      </c>
+      <c r="G2">
+        <f>MIN(B:B)</f>
+        <v>573.55117385851304</v>
+      </c>
+      <c r="H2">
+        <f>MAX(C:C)</f>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>